<commit_message>
Item and order changes
</commit_message>
<xml_diff>
--- a/public/Sample/items_sample.xlsx
+++ b/public/Sample/items_sample.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>location</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>remarks</t>
-  </si>
-  <si>
-    <t>customer_name</t>
   </si>
 </sst>
 </file>
@@ -477,7 +474,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -485,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -500,7 +497,7 @@
     <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
@@ -516,42 +513,39 @@
     <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="G1" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:10">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="1"/>

</xml_diff>